<commit_message>
Commentaires ... mise à jour
</commit_message>
<xml_diff>
--- a/BTS SIO-2025-E5-Tableau de synthese.xlsx
+++ b/BTS SIO-2025-E5-Tableau de synthese.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\portfolionew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{7E912719-FA98-470A-A2AC-09055BFC295F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC1E7B0-6AB6-4E8D-AD87-24596597C25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E5" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E5'!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -86,105 +85,105 @@
     <t>Organiser son développement professionnel</t>
   </si>
   <si>
-    <t>▸Recenser et identifier les ressources numériques 
+    <t>▸Collecter, suivre et orienter des demandes 
+▸Traiter des demandes concernant les services réseau et système, applicatifs
+▸Traiter des demandes concernant les applications</t>
+  </si>
+  <si>
+    <t>▸Participer à la valorisation de l’image de l’organisation sur les médias numériques en tenant compte du cadre juridique et des enjeux économiques
+▸Référencer les services en ligne de l’organisation et mesurer leur visibilité.
+▸Participer à l’évolution d’un site Web exploitant les données de l’organisation.</t>
+  </si>
+  <si>
+    <t>▸Analyser les objectifs et les modalités d’organisation d’un projet
+▸Planifier les activités
+▸Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
+  </si>
+  <si>
+    <t>▸Réaliser les tests d’intégration et d’acceptation d’un service
+▸Déployer un service
+▸Accompagner les utilisateurs dans la mise en place d’un service</t>
+  </si>
+  <si>
+    <t>▸Mettre en place son environnement d’apprentissage personnel
+▸Mettre en œuvre des outils et stratégies de veille informationnelle
+▸Gérer son identité professionnelle
+▸Développer son projet professionnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation en cours de formation
+</t>
+  </si>
+  <si>
+    <t>Réalisations en milieu professionnel en cours de première année</t>
+  </si>
+  <si>
+    <t>Réalisations en milieu professionnel en cours de seconde année</t>
+  </si>
+  <si>
+    <t>Mon professionnel</t>
+  </si>
+  <si>
+    <t>Mon particulier</t>
+  </si>
+  <si>
+    <t>NOM et prénom : Etourmy Quentin</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://portfolio.qetourmy.com/</t>
+  </si>
+  <si>
+    <t>Centre de formation : ESPL</t>
+  </si>
+  <si>
+    <t>Bienvenue Formation</t>
+  </si>
+  <si>
+    <t>clic and eat</t>
+  </si>
+  <si>
+    <t>N° candidat : 2442743787</t>
+  </si>
+  <si>
+    <t>IA AXA</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Portfolio BTS SIO SLAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/2023 -
+06/2024 </t>
+  </si>
+  <si>
+    <t>09/2024 -
+02/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/2024 -
+12/2024 </t>
+  </si>
+  <si>
+    <t>02/2025 -
+03/2025</t>
+  </si>
+  <si>
+    <t>09/2023 -
+04/2025</t>
+  </si>
+  <si>
+    <t>01/2025 -
+06/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">▸Recenser et identifier les ressources numériques 
 ▸Exploiter des référentiels, normes et standards adoptés par le prestataire informatique
 ▸Mettre en place et vérifier les niveaux d’habilitation associés à un service
 ▸Vérifier les conditions de la continuité d’un service informatique
 ▸Gérer des sauvegardes
-▸Vérifier le respect des règles d’utilisation des ressources numériques</t>
-  </si>
-  <si>
-    <t>▸Collecter, suivre et orienter des demandes 
-▸Traiter des demandes concernant les services réseau et système, applicatifs
-▸Traiter des demandes concernant les applications</t>
-  </si>
-  <si>
-    <t>▸Participer à la valorisation de l’image de l’organisation sur les médias numériques en tenant compte du cadre juridique et des enjeux économiques
-▸Référencer les services en ligne de l’organisation et mesurer leur visibilité.
-▸Participer à l’évolution d’un site Web exploitant les données de l’organisation.</t>
-  </si>
-  <si>
-    <t>▸Analyser les objectifs et les modalités d’organisation d’un projet
-▸Planifier les activités
-▸Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
-  </si>
-  <si>
-    <t>▸Réaliser les tests d’intégration et d’acceptation d’un service
-▸Déployer un service
-▸Accompagner les utilisateurs dans la mise en place d’un service</t>
-  </si>
-  <si>
-    <t>▸Mettre en place son environnement d’apprentissage personnel
-▸Mettre en œuvre des outils et stratégies de veille informationnelle
-▸Gérer son identité professionnelle
-▸Développer son projet professionnel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réalisation en cours de formation
 </t>
-  </si>
-  <si>
-    <t>Réalisations en milieu professionnel en cours de première année</t>
-  </si>
-  <si>
-    <t>Réalisations en milieu professionnel en cours de seconde année</t>
-  </si>
-  <si>
-    <t>Mon professionnel</t>
-  </si>
-  <si>
-    <t>Mon particulier</t>
-  </si>
-  <si>
-    <t>NOM et prénom : Etourmy Quentin</t>
-  </si>
-  <si>
-    <t>Adresse URL du portfolio : https://portfolio.qetourmy.com/</t>
-  </si>
-  <si>
-    <t>Centre de formation : ESPL</t>
-  </si>
-  <si>
-    <t>Bienvenue Formation</t>
-  </si>
-  <si>
-    <t>clic and eat</t>
-  </si>
-  <si>
-    <t>N° candidat : 2442743787</t>
-  </si>
-  <si>
-    <t>IA AXA</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Portfolio BTS SIO SLAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/2023 -
-06/2024 </t>
-  </si>
-  <si>
-    <t>09/2024 -
-02/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/2024 -
-12/2024 </t>
-  </si>
-  <si>
-    <t>02/2025 -
-03/2025</t>
-  </si>
-  <si>
-    <t>09/2023 -
-04/2025</t>
-  </si>
-  <si>
-    <t>01/2025 -
-06/2025</t>
   </si>
 </sst>
 </file>
@@ -266,7 +265,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -327,7 +326,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </left>
       <right style="thin">
@@ -345,73 +344,13 @@
       <left style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color theme="2" tint="-0.749992370372631"/>
       </right>
       <top style="medium">
         <color theme="2" tint="-0.749992370372631"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
         <color theme="2" tint="-0.749992370372631"/>
       </bottom>
       <diagonal/>
@@ -471,59 +410,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </left>
       <right style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
       <top style="medium">
         <color theme="2" tint="-0.749992370372631"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -668,12 +564,98 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </left>
       <right style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
       <top style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </top>
@@ -681,8 +663,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color theme="2" tint="-0.749992370372631"/>
@@ -690,6 +672,51 @@
       <top/>
       <bottom style="thin">
         <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -698,7 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -715,24 +742,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -742,40 +760,64 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -784,70 +826,58 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1235,8 +1265,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1275,57 +1305,57 @@
       <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="30"/>
+      <c r="A3" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="35"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="12" t="s">
+      <c r="A4" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="A5" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1347,26 +1377,26 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="19" t="s">
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="E7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="H7" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>19</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1405,16 +1435,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="A8" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1452,25 +1482,25 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>32</v>
+      <c r="A9" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>31</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1509,25 +1539,25 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="45" t="s">
-        <v>32</v>
+      <c r="A10" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>31</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1566,18 +1596,24 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
+      <c r="A11" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>31</v>
+      </c>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1615,14 +1651,14 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="49"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="44"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1660,14 +1696,14 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="44"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1705,14 +1741,14 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="44"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1750,14 +1786,14 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="44"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1795,14 +1831,14 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="44"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1840,14 +1876,14 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="44"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1885,14 +1921,14 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="44"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1930,16 +1966,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="A19" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="47"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1977,24 +2013,24 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="44"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -2032,14 +2068,14 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="44"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -2077,14 +2113,14 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
+      <c r="A22" s="45"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="44"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2122,14 +2158,14 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="44"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2167,14 +2203,14 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
+      <c r="A24" s="45"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="15"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="44"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2212,14 +2248,14 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
+      <c r="A25" s="45"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="44"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2257,14 +2293,14 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
+      <c r="A26" s="45"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="44"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2302,16 +2338,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
+      <c r="A27" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="47"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2349,24 +2385,24 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
+      <c r="A28" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="11"/>
+      <c r="H28" s="44"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2404,20 +2440,20 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="15"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="44"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2455,14 +2491,14 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
+      <c r="A30" s="45"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="44"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2500,14 +2536,14 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
+      <c r="A31" s="45"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="44"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2545,14 +2581,14 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
+      <c r="A32" s="45"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="44"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2590,14 +2626,14 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
+      <c r="A33" s="45"/>
       <c r="B33" s="8"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="44"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2634,15 +2670,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="17"/>
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="48"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="51"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2772,6 +2808,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2779,11 +2820,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2795,26 +2831,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d1edcf93-3b42-4c26-849c-df4ad50c6d74">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fd978a6a-a7ab-40db-b5ff-a45cb379138c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B953A76F76DF4A89A17CC56707788F" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="7f4650baa30b23dbba916b12213459cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d1edcf93-3b42-4c26-849c-df4ad50c6d74" xmlns:ns3="fd978a6a-a7ab-40db-b5ff-a45cb379138c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d7db0278cda2bf964613189477aaf99" ns2:_="" ns3:_="">
     <xsd:import namespace="d1edcf93-3b42-4c26-849c-df4ad50c6d74"/>
@@ -3009,26 +3025,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE625886-430A-48B8-8375-B4C7BE82EC53}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d1edcf93-3b42-4c26-849c-df4ad50c6d74"/>
-    <ds:schemaRef ds:uri="fd978a6a-a7ab-40db-b5ff-a45cb379138c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{745A5F59-39E5-4724-9F13-5E268844DBDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d1edcf93-3b42-4c26-849c-df4ad50c6d74">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fd978a6a-a7ab-40db-b5ff-a45cb379138c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C75BDBBF-A7E0-472B-A860-BBBA38D5CE27}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3045,4 +3062,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{745A5F59-39E5-4724-9F13-5E268844DBDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE625886-430A-48B8-8375-B4C7BE82EC53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d1edcf93-3b42-4c26-849c-df4ad50c6d74"/>
+    <ds:schemaRef ds:uri="fd978a6a-a7ab-40db-b5ff-a45cb379138c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>